<commit_message>
Update with UI refinements and new subtab navigation
</commit_message>
<xml_diff>
--- a/data/cx_dim_callback_reason.xlsx
+++ b/data/cx_dim_callback_reason.xlsx
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>call_back_reason_id</t>
+          <t>callback_reason_id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>call_back_reason</t>
+          <t>callback_reason</t>
         </is>
       </c>
     </row>

</xml_diff>